<commit_message>
Cotejo escaleta y recursos en greco
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/Escaleta MA_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/Escaleta MA_07_01_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -957,7 +957,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1039,6 +1039,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1200,7 +1206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1456,6 +1462,33 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1477,6 +1510,9 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1486,35 +1522,8 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6108,8 +6117,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JX67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="26.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6140,13 +6149,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:284" s="38" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A1" s="108" t="s">
+      <c r="A1" s="117" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="122" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="35" t="s">
@@ -6158,47 +6167,47 @@
       <c r="F1" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="G1" s="118" t="s">
+      <c r="G1" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="110" t="s">
+      <c r="H1" s="119" t="s">
         <v>242</v>
       </c>
-      <c r="I1" s="109" t="s">
+      <c r="I1" s="118" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="110" t="s">
+      <c r="J1" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="113" t="s">
+      <c r="K1" s="123" t="s">
         <v>243</v>
       </c>
-      <c r="L1" s="109" t="s">
+      <c r="L1" s="118" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="111" t="s">
+      <c r="M1" s="120" t="s">
         <v>25</v>
       </c>
-      <c r="N1" s="111"/>
-      <c r="O1" s="105" t="s">
+      <c r="N1" s="120"/>
+      <c r="O1" s="114" t="s">
         <v>102</v>
       </c>
-      <c r="P1" s="107" t="s">
+      <c r="P1" s="116" t="s">
         <v>103</v>
       </c>
-      <c r="Q1" s="115" t="s">
+      <c r="Q1" s="111" t="s">
         <v>89</v>
       </c>
-      <c r="R1" s="117" t="s">
+      <c r="R1" s="113" t="s">
         <v>90</v>
       </c>
-      <c r="S1" s="115" t="s">
+      <c r="S1" s="111" t="s">
         <v>91</v>
       </c>
-      <c r="T1" s="116" t="s">
+      <c r="T1" s="112" t="s">
         <v>92</v>
       </c>
-      <c r="U1" s="115" t="s">
+      <c r="U1" s="111" t="s">
         <v>93</v>
       </c>
       <c r="V1" s="37"/>
@@ -6467,9 +6476,9 @@
       <c r="JX1" s="39"/>
     </row>
     <row r="2" spans="1:284" s="38" customFormat="1" ht="12" x14ac:dyDescent="0.2">
-      <c r="A2" s="108"/>
-      <c r="B2" s="106"/>
-      <c r="C2" s="112"/>
+      <c r="A2" s="117"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="122"/>
       <c r="D2" s="35" t="s">
         <v>178</v>
       </c>
@@ -6479,25 +6488,25 @@
       <c r="F2" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="G2" s="118"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="114"/>
-      <c r="L2" s="109"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="118"/>
       <c r="M2" s="41" t="s">
         <v>94</v>
       </c>
       <c r="N2" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="O2" s="105"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="115"/>
-      <c r="R2" s="117"/>
-      <c r="S2" s="115"/>
-      <c r="T2" s="116"/>
-      <c r="U2" s="115"/>
+      <c r="O2" s="114"/>
+      <c r="P2" s="116"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="111"/>
       <c r="V2" s="37"/>
       <c r="X2" s="39"/>
       <c r="Y2" s="39"/>
@@ -6778,7 +6787,7 @@
       </c>
       <c r="E3" s="93"/>
       <c r="F3" s="93"/>
-      <c r="G3" s="119" t="s">
+      <c r="G3" s="105" t="s">
         <v>123</v>
       </c>
       <c r="H3" s="93">
@@ -6843,7 +6852,7 @@
         <v>127</v>
       </c>
       <c r="F4" s="93"/>
-      <c r="G4" s="119" t="s">
+      <c r="G4" s="105" t="s">
         <v>128</v>
       </c>
       <c r="H4" s="101">
@@ -6908,7 +6917,7 @@
         <v>225</v>
       </c>
       <c r="F5" s="93"/>
-      <c r="G5" s="119" t="s">
+      <c r="G5" s="105" t="s">
         <v>195</v>
       </c>
       <c r="H5" s="101">
@@ -6973,7 +6982,7 @@
         <v>129</v>
       </c>
       <c r="F6" s="35"/>
-      <c r="G6" s="120" t="s">
+      <c r="G6" s="106" t="s">
         <v>194</v>
       </c>
       <c r="H6" s="51">
@@ -7299,7 +7308,7 @@
         <v>129</v>
       </c>
       <c r="F7" s="35"/>
-      <c r="G7" s="120" t="s">
+      <c r="G7" s="106" t="s">
         <v>160</v>
       </c>
       <c r="H7" s="51">
@@ -7945,7 +7954,7 @@
         <v>130</v>
       </c>
       <c r="F9" s="93"/>
-      <c r="G9" s="119" t="s">
+      <c r="G9" s="125" t="s">
         <v>204</v>
       </c>
       <c r="H9" s="93">
@@ -8010,7 +8019,7 @@
         <v>130</v>
       </c>
       <c r="F10" s="93"/>
-      <c r="G10" s="119" t="s">
+      <c r="G10" s="105" t="s">
         <v>206</v>
       </c>
       <c r="H10" s="93">
@@ -8073,7 +8082,7 @@
         <v>110</v>
       </c>
       <c r="F11" s="35"/>
-      <c r="G11" s="120" t="s">
+      <c r="G11" s="106" t="s">
         <v>249</v>
       </c>
       <c r="H11" s="51">
@@ -8396,7 +8405,7 @@
       </c>
       <c r="E12" s="36"/>
       <c r="F12" s="35"/>
-      <c r="G12" s="120" t="s">
+      <c r="G12" s="106" t="s">
         <v>250</v>
       </c>
       <c r="H12" s="51">
@@ -8715,7 +8724,7 @@
       <c r="F13" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="G13" s="120" t="s">
+      <c r="G13" s="106" t="s">
         <v>146</v>
       </c>
       <c r="H13" s="51">
@@ -9355,7 +9364,7 @@
       </c>
       <c r="E15" s="36"/>
       <c r="F15" s="35"/>
-      <c r="G15" s="120" t="s">
+      <c r="G15" s="106" t="s">
         <v>135</v>
       </c>
       <c r="H15" s="51">
@@ -9678,7 +9687,7 @@
       </c>
       <c r="E16" s="36"/>
       <c r="F16" s="35"/>
-      <c r="G16" s="120" t="s">
+      <c r="G16" s="106" t="s">
         <v>136</v>
       </c>
       <c r="H16" s="51">
@@ -10001,7 +10010,7 @@
       </c>
       <c r="E17" s="36"/>
       <c r="F17" s="35"/>
-      <c r="G17" s="120" t="s">
+      <c r="G17" s="106" t="s">
         <v>134</v>
       </c>
       <c r="H17" s="51">
@@ -10324,7 +10333,7 @@
       </c>
       <c r="E18" s="36"/>
       <c r="F18" s="35"/>
-      <c r="G18" s="120" t="s">
+      <c r="G18" s="106" t="s">
         <v>214</v>
       </c>
       <c r="H18" s="51">
@@ -10641,7 +10650,7 @@
         <v>110</v>
       </c>
       <c r="F19" s="35"/>
-      <c r="G19" s="120" t="s">
+      <c r="G19" s="106" t="s">
         <v>229</v>
       </c>
       <c r="H19" s="44">
@@ -10964,7 +10973,7 @@
       </c>
       <c r="E20" s="36"/>
       <c r="F20" s="35"/>
-      <c r="G20" s="120" t="s">
+      <c r="G20" s="106" t="s">
         <v>217</v>
       </c>
       <c r="H20" s="44">
@@ -11283,14 +11292,14 @@
         <v>226</v>
       </c>
       <c r="F21" s="35"/>
-      <c r="G21" s="120" t="s">
+      <c r="G21" s="106" t="s">
         <v>223</v>
       </c>
       <c r="H21" s="44">
         <v>19</v>
       </c>
       <c r="I21" s="52"/>
-      <c r="J21" s="124"/>
+      <c r="J21" s="110"/>
       <c r="K21" s="45" t="s">
         <v>115</v>
       </c>
@@ -11604,7 +11613,7 @@
       <c r="F22" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="G22" s="120" t="s">
+      <c r="G22" s="106" t="s">
         <v>143</v>
       </c>
       <c r="H22" s="51">
@@ -11929,7 +11938,7 @@
         <v>148</v>
       </c>
       <c r="F23" s="35"/>
-      <c r="G23" s="120" t="s">
+      <c r="G23" s="106" t="s">
         <v>149</v>
       </c>
       <c r="H23" s="51">
@@ -12254,7 +12263,7 @@
         <v>148</v>
       </c>
       <c r="F24" s="35"/>
-      <c r="G24" s="120" t="s">
+      <c r="G24" s="106" t="s">
         <v>151</v>
       </c>
       <c r="H24" s="51">
@@ -12579,7 +12588,7 @@
         <v>148</v>
       </c>
       <c r="F25" s="35"/>
-      <c r="G25" s="120" t="s">
+      <c r="G25" s="106" t="s">
         <v>224</v>
       </c>
       <c r="H25" s="51">
@@ -12904,7 +12913,7 @@
         <v>110</v>
       </c>
       <c r="F26" s="35"/>
-      <c r="G26" s="120" t="s">
+      <c r="G26" s="106" t="s">
         <v>248</v>
       </c>
       <c r="H26" s="44">
@@ -13227,7 +13236,7 @@
       </c>
       <c r="E27" s="36"/>
       <c r="F27" s="35"/>
-      <c r="G27" s="121" t="s">
+      <c r="G27" s="107" t="s">
         <v>230</v>
       </c>
       <c r="H27" s="51">
@@ -13550,7 +13559,7 @@
       </c>
       <c r="E28" s="36"/>
       <c r="F28" s="35"/>
-      <c r="G28" s="120" t="s">
+      <c r="G28" s="106" t="s">
         <v>236</v>
       </c>
       <c r="H28" s="51">
@@ -13875,7 +13884,7 @@
         <v>14</v>
       </c>
       <c r="F29" s="35"/>
-      <c r="G29" s="120"/>
+      <c r="G29" s="106"/>
       <c r="H29" s="51">
         <v>28</v>
       </c>
@@ -14176,7 +14185,7 @@
         <v>157</v>
       </c>
       <c r="F30" s="35"/>
-      <c r="G30" s="120"/>
+      <c r="G30" s="106"/>
       <c r="H30" s="51">
         <v>29</v>
       </c>
@@ -14230,7 +14239,7 @@
       </c>
       <c r="E31" s="36"/>
       <c r="F31" s="35"/>
-      <c r="G31" s="120"/>
+      <c r="G31" s="106"/>
       <c r="H31" s="51"/>
       <c r="I31" s="52"/>
       <c r="J31" s="53"/>
@@ -14254,7 +14263,7 @@
       <c r="B32" s="62"/>
       <c r="C32" s="63"/>
       <c r="D32" s="64"/>
-      <c r="G32" s="122"/>
+      <c r="G32" s="108"/>
       <c r="H32" s="68"/>
       <c r="I32" s="67"/>
       <c r="J32" s="69"/>
@@ -14276,7 +14285,7 @@
       <c r="B33" s="65"/>
       <c r="C33" s="63"/>
       <c r="D33" s="76"/>
-      <c r="G33" s="123"/>
+      <c r="G33" s="109"/>
       <c r="H33" s="78"/>
       <c r="I33" s="77"/>
       <c r="J33" s="79"/>
@@ -14298,7 +14307,7 @@
       <c r="B34" s="65"/>
       <c r="C34" s="63"/>
       <c r="D34" s="76"/>
-      <c r="G34" s="123"/>
+      <c r="G34" s="109"/>
       <c r="H34" s="78"/>
       <c r="I34" s="77"/>
       <c r="J34" s="79"/>
@@ -14320,7 +14329,7 @@
       <c r="B35" s="65"/>
       <c r="C35" s="63"/>
       <c r="D35" s="76"/>
-      <c r="G35" s="123"/>
+      <c r="G35" s="109"/>
       <c r="H35" s="78"/>
       <c r="I35" s="77"/>
       <c r="J35" s="79"/>
@@ -14342,7 +14351,7 @@
       <c r="B36" s="65"/>
       <c r="C36" s="63"/>
       <c r="D36" s="76"/>
-      <c r="G36" s="123"/>
+      <c r="G36" s="109"/>
       <c r="H36" s="78"/>
       <c r="I36" s="77"/>
       <c r="J36" s="79"/>
@@ -14364,7 +14373,7 @@
       <c r="B37" s="65"/>
       <c r="C37" s="63"/>
       <c r="D37" s="76"/>
-      <c r="G37" s="123"/>
+      <c r="G37" s="109"/>
       <c r="H37" s="78"/>
       <c r="I37" s="77"/>
       <c r="J37" s="79"/>
@@ -14385,7 +14394,7 @@
       <c r="B38" s="82"/>
       <c r="C38" s="83"/>
       <c r="D38" s="76"/>
-      <c r="G38" s="123"/>
+      <c r="G38" s="109"/>
       <c r="H38" s="78"/>
       <c r="I38" s="77"/>
       <c r="J38" s="79"/>
@@ -14406,7 +14415,7 @@
       <c r="B39" s="82"/>
       <c r="C39" s="83"/>
       <c r="D39" s="76"/>
-      <c r="G39" s="123"/>
+      <c r="G39" s="109"/>
       <c r="H39" s="78"/>
       <c r="I39" s="77"/>
       <c r="J39" s="79"/>
@@ -14427,7 +14436,7 @@
       <c r="B40" s="82"/>
       <c r="C40" s="83"/>
       <c r="D40" s="76"/>
-      <c r="G40" s="123"/>
+      <c r="G40" s="109"/>
       <c r="H40" s="78"/>
       <c r="I40" s="77"/>
       <c r="J40" s="79"/>
@@ -14448,7 +14457,7 @@
       <c r="B41" s="82"/>
       <c r="C41" s="83"/>
       <c r="D41" s="76"/>
-      <c r="G41" s="123"/>
+      <c r="G41" s="109"/>
       <c r="H41" s="78"/>
       <c r="I41" s="77"/>
       <c r="J41" s="79"/>
@@ -14469,7 +14478,7 @@
       <c r="B42" s="82"/>
       <c r="C42" s="83"/>
       <c r="D42" s="76"/>
-      <c r="G42" s="123"/>
+      <c r="G42" s="109"/>
       <c r="H42" s="78"/>
       <c r="I42" s="77"/>
       <c r="J42" s="79"/>
@@ -14490,7 +14499,7 @@
       <c r="B43" s="82"/>
       <c r="C43" s="83"/>
       <c r="D43" s="76"/>
-      <c r="G43" s="123"/>
+      <c r="G43" s="109"/>
       <c r="H43" s="78"/>
       <c r="I43" s="77"/>
       <c r="J43" s="79"/>
@@ -14511,7 +14520,7 @@
       <c r="B44" s="82"/>
       <c r="C44" s="83"/>
       <c r="D44" s="76"/>
-      <c r="G44" s="123"/>
+      <c r="G44" s="109"/>
       <c r="H44" s="78"/>
       <c r="I44" s="77"/>
       <c r="J44" s="79"/>
@@ -14532,7 +14541,7 @@
       <c r="B45" s="82"/>
       <c r="C45" s="83"/>
       <c r="D45" s="76"/>
-      <c r="G45" s="123"/>
+      <c r="G45" s="109"/>
       <c r="H45" s="78"/>
       <c r="I45" s="77"/>
       <c r="J45" s="79"/>
@@ -14553,7 +14562,7 @@
       <c r="B46" s="82"/>
       <c r="C46" s="83"/>
       <c r="D46" s="76"/>
-      <c r="G46" s="123"/>
+      <c r="G46" s="109"/>
       <c r="H46" s="78"/>
       <c r="I46" s="77"/>
       <c r="J46" s="79"/>
@@ -14574,7 +14583,7 @@
       <c r="B47" s="82"/>
       <c r="C47" s="83"/>
       <c r="D47" s="76"/>
-      <c r="G47" s="123"/>
+      <c r="G47" s="109"/>
       <c r="H47" s="78"/>
       <c r="I47" s="77"/>
       <c r="J47" s="79"/>
@@ -14605,11 +14614,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="P1:P2"/>
@@ -14622,6 +14626,11 @@
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="K1:K2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K31:K47">

</xml_diff>